<commit_message>
LSR now sends an email to me with the first tab of expiring software license info. Need to do the rest of the tabs as well as add headers so it doesn't go to Junk
</commit_message>
<xml_diff>
--- a/lsapRenewal.xlsx
+++ b/lsapRenewal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrisp\Desktop\Chris' Files\Scripts\LSAP renewal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45CD9C4-5A2D-4815-9F7F-F9CDF2D9EE4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D330334F-B099-4DF2-B127-63E6E8693307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{5F82C22A-25CB-4AD9-A3D3-160B82C51E9E}"/>
   </bookViews>
@@ -1599,7 +1599,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1621,7 +1621,7 @@
     <row r="1" spans="1:13" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="33">
         <f ca="1">TODAY()</f>
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -5941,21 +5941,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100947930F0753D384D810E54E3EE41794A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2f0c7ca6c9e3282ba1e3393238566ce7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6c95d2b4-dd8e-4a18-8d6e-79794781b340" xmlns:ns3="946b5ff5-d270-4231-9d11-b30bca1ea5c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54acdf2ad564b6e18a2d1b953374064e" ns2:_="" ns3:_="">
     <xsd:import namespace="6c95d2b4-dd8e-4a18-8d6e-79794781b340"/>
@@ -6132,32 +6117,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7B9CAF7-6FA7-4757-BBAF-E15750B1E271}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="6c95d2b4-dd8e-4a18-8d6e-79794781b340"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="946b5ff5-d270-4231-9d11-b30bca1ea5c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FF0B02-80D7-4AFB-ADEB-812A5A4C2683}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4B2DE20-CB89-4302-AD08-3A0EAB275549}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6174,4 +6149,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FF0B02-80D7-4AFB-ADEB-812A5A4C2683}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7B9CAF7-6FA7-4757-BBAF-E15750B1E271}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="6c95d2b4-dd8e-4a18-8d6e-79794781b340"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="946b5ff5-d270-4231-9d11-b30bca1ea5c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
LSR now scans all the tabs and sends an email with everything as expected.  The only issue left is making it not send to junk mail. working with Jasmeet on that
</commit_message>
<xml_diff>
--- a/lsapRenewal.xlsx
+++ b/lsapRenewal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrisp\Desktop\Chris' Files\Scripts\LSAP renewal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D330334F-B099-4DF2-B127-63E6E8693307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889C60D7-E099-4E0A-956C-BD813A73BCDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{5F82C22A-25CB-4AD9-A3D3-160B82C51E9E}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="7" activeTab="18" xr2:uid="{5F82C22A-25CB-4AD9-A3D3-160B82C51E9E}"/>
   </bookViews>
   <sheets>
     <sheet name="LF" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="353">
   <si>
     <t>Company</t>
   </si>
@@ -1087,12 +1087,6 @@
   </si>
   <si>
     <t>Nothing back from Stephan. Physical Mail.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer </t>
-  </si>
-  <si>
-    <t>Kodak Device</t>
   </si>
   <si>
     <t>Kodak Cap Pro E 5yr Asur/Asist</t>
@@ -1596,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7988D7E7-3335-4EDE-A851-F3E96F7EAB5E}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,7 +1627,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>3</v>
@@ -1665,7 +1659,7 @@
         <v>44003</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1742,7 +1736,7 @@
         <v>43784</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F6" s="18"/>
     </row>
@@ -1760,7 +1754,7 @@
         <v>43784</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>15</v>
@@ -2063,6 +2057,12 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="15"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="16">
+        <f ca="1">COUNT(A1:A24)</f>
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J28">
@@ -2700,7 +2700,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2778,7 +2778,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A2" sqref="A2:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2819,6 +2819,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>290</v>
       </c>
@@ -2840,6 +2843,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>294</v>
       </c>
@@ -2861,6 +2867,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>298</v>
       </c>
@@ -2879,6 +2888,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>300</v>
       </c>
@@ -2900,6 +2912,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>300</v>
       </c>
@@ -2918,6 +2933,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>300</v>
       </c>
@@ -2936,6 +2954,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>304</v>
       </c>
@@ -2954,6 +2975,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>305</v>
       </c>
@@ -2975,6 +2999,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>309</v>
       </c>
@@ -2993,6 +3020,9 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>312</v>
       </c>
@@ -3014,6 +3044,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>315</v>
       </c>
@@ -3032,6 +3065,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>188</v>
       </c>
@@ -3050,6 +3086,9 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>319</v>
       </c>
@@ -3068,6 +3107,9 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>321</v>
       </c>
@@ -3086,6 +3128,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>324</v>
       </c>
@@ -3103,7 +3148,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>326</v>
       </c>
@@ -3121,7 +3169,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
         <v>326</v>
       </c>
@@ -3139,7 +3190,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19" t="s">
         <v>328</v>
       </c>
@@ -3160,7 +3214,10 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>266</v>
       </c>
@@ -3181,7 +3238,10 @@
         <v>333</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>334</v>
       </c>
@@ -3202,7 +3262,10 @@
         <v>336</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>337</v>
       </c>
@@ -3220,7 +3283,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>339</v>
       </c>
@@ -3238,7 +3304,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="B24" t="s">
         <v>339</v>
       </c>
@@ -3256,7 +3325,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
       <c r="B25" t="s">
         <v>341</v>
       </c>
@@ -3277,7 +3349,10 @@
         <v>342</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="B26" t="s">
         <v>341</v>
       </c>
@@ -3295,7 +3370,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
       <c r="B27" t="s">
         <v>343</v>
       </c>
@@ -3313,336 +3391,449 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B22845-B803-4E0B-8CD3-914C2E34E443}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="14" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="33">
+        <f ca="1">TODAY()</f>
+        <v>43767</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" s="12">
+        <v>42446</v>
+      </c>
+      <c r="E2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D3" s="12">
+        <v>41249</v>
+      </c>
+      <c r="E3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="12">
+        <v>42277</v>
+      </c>
+      <c r="E4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D5" s="12">
+        <v>41535</v>
+      </c>
+      <c r="E5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" s="12">
+        <v>41535</v>
+      </c>
+      <c r="E6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D7" s="12">
+        <v>41589</v>
+      </c>
+      <c r="E7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D8" s="12">
+        <v>42444</v>
+      </c>
+      <c r="E8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" s="12">
+        <v>40946</v>
+      </c>
+      <c r="E9" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>309</v>
+      </c>
+      <c r="D10" s="12">
+        <v>41361</v>
+      </c>
+      <c r="E10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>312</v>
+      </c>
+      <c r="D11" s="12">
+        <v>42696</v>
+      </c>
+      <c r="E11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D12" s="12">
+        <v>42696</v>
+      </c>
+      <c r="E12" t="s">
         <v>345</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D13" s="12">
+        <v>42026</v>
+      </c>
+      <c r="E13" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="12">
+        <v>41955</v>
+      </c>
+      <c r="E14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>319</v>
+      </c>
+      <c r="D15" s="12">
+        <v>42181</v>
+      </c>
+      <c r="E15" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>321</v>
+      </c>
+      <c r="D16" s="12">
+        <v>40991</v>
+      </c>
+      <c r="E16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>346</v>
       </c>
-      <c r="C1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C2" s="12">
-        <v>42446</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>294</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D17" s="12">
+        <v>42207</v>
+      </c>
+      <c r="E17" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>324</v>
+      </c>
+      <c r="D18" s="12">
+        <v>40940</v>
+      </c>
+      <c r="E18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>326</v>
+      </c>
+      <c r="D19" s="12">
+        <v>42464</v>
+      </c>
+      <c r="E19" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="12">
-        <v>41249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>326</v>
+      </c>
+      <c r="D20" s="12">
+        <v>42464</v>
+      </c>
+      <c r="E20" t="s">
         <v>295</v>
       </c>
-      <c r="C4" s="12">
-        <v>42277</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>300</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>328</v>
+      </c>
+      <c r="D21" s="12">
+        <v>42577</v>
+      </c>
+      <c r="E21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="12">
+        <v>41375</v>
+      </c>
+      <c r="E22" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>334</v>
+      </c>
+      <c r="D23" s="12">
+        <v>41542</v>
+      </c>
+      <c r="E23" t="s">
         <v>301</v>
       </c>
-      <c r="C5" s="12">
-        <v>41535</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>337</v>
+      </c>
+      <c r="D24" s="12">
+        <v>41150</v>
+      </c>
+      <c r="E24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>339</v>
+      </c>
+      <c r="D25" s="12">
+        <v>41390</v>
+      </c>
+      <c r="E25" t="s">
         <v>301</v>
       </c>
-      <c r="C6" s="12">
-        <v>41535</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>300</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>339</v>
+      </c>
+      <c r="D26" s="12">
+        <v>41390</v>
+      </c>
+      <c r="E26" t="s">
         <v>301</v>
       </c>
-      <c r="C7" s="12">
-        <v>41589</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>304</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>341</v>
+      </c>
+      <c r="D27" s="12">
+        <v>41718</v>
+      </c>
+      <c r="E27" t="s">
         <v>301</v>
       </c>
-      <c r="C8" s="12">
-        <v>42444</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>305</v>
-      </c>
-      <c r="B9" t="s">
-        <v>306</v>
-      </c>
-      <c r="C9" s="12">
-        <v>40946</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>309</v>
-      </c>
-      <c r="B10" t="s">
-        <v>310</v>
-      </c>
-      <c r="C10" s="12">
-        <v>41361</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C11" s="12">
-        <v>42696</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>312</v>
-      </c>
-      <c r="B12" t="s">
-        <v>347</v>
-      </c>
-      <c r="C12" s="12">
-        <v>42696</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>315</v>
-      </c>
-      <c r="B13" t="s">
-        <v>316</v>
-      </c>
-      <c r="C13" s="12">
-        <v>42026</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14" t="s">
-        <v>310</v>
-      </c>
-      <c r="C14" s="12">
-        <v>41955</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>319</v>
-      </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>341</v>
+      </c>
+      <c r="D28" s="12">
+        <v>41718</v>
+      </c>
+      <c r="E28" t="s">
         <v>301</v>
       </c>
-      <c r="C15" s="12">
-        <v>42181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>321</v>
-      </c>
-      <c r="B16" t="s">
-        <v>322</v>
-      </c>
-      <c r="C16" s="12">
-        <v>40991</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>341</v>
+      </c>
+      <c r="D29" s="12">
+        <v>41891</v>
+      </c>
+      <c r="E29" t="s">
         <v>348</v>
-      </c>
-      <c r="B17" t="s">
-        <v>349</v>
-      </c>
-      <c r="C17" s="12">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>324</v>
-      </c>
-      <c r="B18" t="s">
-        <v>306</v>
-      </c>
-      <c r="C18" s="12">
-        <v>40940</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>326</v>
-      </c>
-      <c r="B19" t="s">
-        <v>295</v>
-      </c>
-      <c r="C19" s="12">
-        <v>42464</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>326</v>
-      </c>
-      <c r="B20" t="s">
-        <v>295</v>
-      </c>
-      <c r="C20" s="12">
-        <v>42464</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>328</v>
-      </c>
-      <c r="B21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C21" s="12">
-        <v>42577</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>266</v>
-      </c>
-      <c r="B22" t="s">
-        <v>331</v>
-      </c>
-      <c r="C22" s="12">
-        <v>41375</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>334</v>
-      </c>
-      <c r="B23" t="s">
-        <v>301</v>
-      </c>
-      <c r="C23" s="12">
-        <v>41542</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>337</v>
-      </c>
-      <c r="B24" t="s">
-        <v>310</v>
-      </c>
-      <c r="C24" s="12">
-        <v>41150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>339</v>
-      </c>
-      <c r="B25" t="s">
-        <v>301</v>
-      </c>
-      <c r="C25" s="12">
-        <v>41390</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>339</v>
-      </c>
-      <c r="B26" t="s">
-        <v>301</v>
-      </c>
-      <c r="C26" s="12">
-        <v>41390</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>341</v>
-      </c>
-      <c r="B27" t="s">
-        <v>301</v>
-      </c>
-      <c r="C27" s="12">
-        <v>41718</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>341</v>
-      </c>
-      <c r="B28" t="s">
-        <v>301</v>
-      </c>
-      <c r="C28" s="12">
-        <v>41718</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>341</v>
-      </c>
-      <c r="B29" t="s">
-        <v>350</v>
-      </c>
-      <c r="C29" s="12">
-        <v>41891</v>
       </c>
     </row>
   </sheetData>
@@ -3655,12 +3846,12 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="16" customWidth="1"/>
     <col min="2" max="2" width="35.88671875" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.6640625" style="16" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
@@ -6118,18 +6309,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6152,14 +6343,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FF0B02-80D7-4AFB-ADEB-812A5A4C2683}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7B9CAF7-6FA7-4757-BBAF-E15750B1E271}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -6174,4 +6357,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FF0B02-80D7-4AFB-ADEB-812A5A4C2683}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cleaned up some debug statements and commented code
</commit_message>
<xml_diff>
--- a/lsapRenewal.xlsx
+++ b/lsapRenewal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrisp\Desktop\Chris' Files\Scripts\LSAP renewal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889C60D7-E099-4E0A-956C-BD813A73BCDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B301F0D-C184-40EF-93A0-AF20E5109D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="7" activeTab="18" xr2:uid="{5F82C22A-25CB-4AD9-A3D3-160B82C51E9E}"/>
   </bookViews>
@@ -3394,7 +3394,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changed header info trying to get out of spam folder. not working yet
</commit_message>
<xml_diff>
--- a/lsapRenewal.xlsx
+++ b/lsapRenewal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrisp\Desktop\Chris' Files\Scripts\LSAP renewal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B301F0D-C184-40EF-93A0-AF20E5109D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699A9817-FA44-47A5-8DFA-F251D588EF0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="7" activeTab="18" xr2:uid="{5F82C22A-25CB-4AD9-A3D3-160B82C51E9E}"/>
+    <workbookView xWindow="-14700" yWindow="0" windowWidth="11070" windowHeight="5730" firstSheet="7" activeTab="18" xr2:uid="{5F82C22A-25CB-4AD9-A3D3-160B82C51E9E}"/>
   </bookViews>
   <sheets>
     <sheet name="LF" sheetId="1" r:id="rId1"/>
@@ -1615,7 +1615,7 @@
     <row r="1" spans="1:13" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="33">
         <f ca="1">TODAY()</f>
-        <v>43767</v>
+        <v>43769</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -3394,7 +3394,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3414,7 +3414,7 @@
     <row r="1" spans="1:10" s="14" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="33">
         <f ca="1">TODAY()</f>
-        <v>43767</v>
+        <v>43769</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -6309,18 +6309,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6343,6 +6343,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FF0B02-80D7-4AFB-ADEB-812A5A4C2683}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7B9CAF7-6FA7-4757-BBAF-E15750B1E271}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -6357,12 +6365,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FF0B02-80D7-4AFB-ADEB-812A5A4C2683}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>